<commit_message>
Added end-to-end Prepoc example
</commit_message>
<xml_diff>
--- a/image_preprocessing/two_vertex/accuracy_degradation/physical/image_classification.xlsx
+++ b/image_preprocessing/two_vertex/accuracy_degradation/physical/image_classification.xlsx
@@ -529,7 +529,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>72.40000000000001</v>
+        <v>75.8</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -643,10 +643,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>20.51681041717529</v>
+        <v>20.45356750488281</v>
       </c>
       <c r="G4" t="n">
-        <v>113.3398035564177</v>
+        <v>117.1840430034826</v>
       </c>
     </row>
     <row r="5">
@@ -672,10 +672,10 @@
         <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>31.067214012146</v>
+        <v>31.36816978454589</v>
       </c>
       <c r="G5" t="n">
-        <v>138.5242222134738</v>
+        <v>156.5747949575072</v>
       </c>
     </row>
     <row r="6">
@@ -701,10 +701,10 @@
         <v>4</v>
       </c>
       <c r="F6" t="n">
-        <v>55.74678182601928</v>
+        <v>51.50646448135375</v>
       </c>
       <c r="G6" t="n">
-        <v>134.0521982008264</v>
+        <v>156.7974428542034</v>
       </c>
     </row>
     <row r="7">
@@ -730,10 +730,10 @@
         <v>8</v>
       </c>
       <c r="F7" t="n">
-        <v>101.177773475647</v>
+        <v>100.9795737266541</v>
       </c>
       <c r="G7" t="n">
-        <v>128.2951477483478</v>
+        <v>140.3298589991225</v>
       </c>
     </row>
     <row r="8">
@@ -759,10 +759,10 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>28.595871925354</v>
+        <v>29.50067996978759</v>
       </c>
       <c r="G8" t="n">
-        <v>78.80772590427378</v>
+        <v>78.5649895349803</v>
       </c>
     </row>
     <row r="9">
@@ -788,10 +788,10 @@
         <v>2</v>
       </c>
       <c r="F9" t="n">
-        <v>32.94711351394653</v>
+        <v>31.62540197372437</v>
       </c>
       <c r="G9" t="n">
-        <v>128.618489766525</v>
+        <v>127.264902264969</v>
       </c>
     </row>
     <row r="10">
@@ -817,10 +817,10 @@
         <v>4</v>
       </c>
       <c r="F10" t="n">
-        <v>37.57479906082153</v>
+        <v>37.55554676055907</v>
       </c>
       <c r="G10" t="n">
-        <v>179.4806751749917</v>
+        <v>176.3530181846559</v>
       </c>
     </row>
     <row r="11">
@@ -846,10 +846,10 @@
         <v>8</v>
       </c>
       <c r="F11" t="n">
-        <v>54.17595386505125</v>
+        <v>51.32622241973876</v>
       </c>
       <c r="G11" t="n">
-        <v>166.9312405371692</v>
+        <v>219.2586291672717</v>
       </c>
     </row>
     <row r="12">
@@ -875,10 +875,10 @@
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>19.89426136016846</v>
+        <v>19.88508224487304</v>
       </c>
       <c r="G12" t="n">
-        <v>118.3118522902629</v>
+        <v>107.7219149462287</v>
       </c>
     </row>
     <row r="13">
@@ -904,10 +904,10 @@
         <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>30.62334775924682</v>
+        <v>31.80617332458496</v>
       </c>
       <c r="G13" t="n">
-        <v>157.6693986780639</v>
+        <v>141.0505317091839</v>
       </c>
     </row>
     <row r="14">
@@ -933,10 +933,10 @@
         <v>4</v>
       </c>
       <c r="F14" t="n">
-        <v>54.12736415863037</v>
+        <v>51.76976203918457</v>
       </c>
       <c r="G14" t="n">
-        <v>164.0259900953315</v>
+        <v>137.396714248651</v>
       </c>
     </row>
     <row r="15">
@@ -962,10 +962,10 @@
         <v>8</v>
       </c>
       <c r="F15" t="n">
-        <v>96.48118734359741</v>
+        <v>98.14545869827271</v>
       </c>
       <c r="G15" t="n">
-        <v>150.1003531003389</v>
+        <v>133.8823067660375</v>
       </c>
     </row>
     <row r="16">
@@ -991,10 +991,10 @@
         <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>25.29911756515503</v>
+        <v>24.84185218811035</v>
       </c>
       <c r="G16" t="n">
-        <v>97.03822580153341</v>
+        <v>97.08632510682425</v>
       </c>
     </row>
     <row r="17">
@@ -1020,10 +1020,10 @@
         <v>2</v>
       </c>
       <c r="F17" t="n">
-        <v>26.91932916641235</v>
+        <v>28.20687532424926</v>
       </c>
       <c r="G17" t="n">
-        <v>147.0392391028999</v>
+        <v>139.4325870695722</v>
       </c>
     </row>
     <row r="18">
@@ -1049,10 +1049,10 @@
         <v>4</v>
       </c>
       <c r="F18" t="n">
-        <v>33.29339265823364</v>
+        <v>33.45731496810912</v>
       </c>
       <c r="G18" t="n">
-        <v>180.975479470437</v>
+        <v>171.55825862255</v>
       </c>
     </row>
     <row r="19">
@@ -1078,10 +1078,10 @@
         <v>8</v>
       </c>
       <c r="F19" t="n">
-        <v>43.86476755142211</v>
+        <v>50.9054136276245</v>
       </c>
       <c r="G19" t="n">
-        <v>210.3419770231335</v>
+        <v>225.5949406713249</v>
       </c>
     </row>
   </sheetData>
@@ -1154,7 +1154,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{"Classifier-resnet50/prepoc-resnet50": {"CPU1": {"THROUGHPUT": [[1, 113.33980355641768], [2, 138.5242222134738], [4, 134.05219820082644], [8, 128.29514774834783]], "LATENCY": [[1, 20.516810417175293], [2, 31.067214012145996], [4, 55.74678182601928], [8, 101.17777347564697]]}}, "Classifier-resnet50/model-resnet50": {"Tesla P40": {"THROUGHPUT": [[1, 78.80772590427378], [2, 128.618489766525], [4, 179.48067517499166], [8, 166.9312405371692]], "LATENCY": [[1, 28.595871925354004], [2, 32.947113513946526], [4, 37.574799060821526], [8, 54.17595386505125]]}}}</t>
+          <t>{"Classifier-resnet50/prepoc-resnet50": {"CPU1": {"THROUGHPUT": [[1, 117.18404300348257], [2, 156.57479495750724], [4, 156.79744285420344], [8, 140.32985899912248]], "LATENCY": [[1, 20.45356750488281], [2, 31.368169784545895], [4, 51.50646448135375], [8, 100.97957372665405]]}}, "Classifier-resnet50/model-resnet50": {"Tesla P40": {"THROUGHPUT": [[1, 78.5649895349803], [2, 127.26490226496902], [4, 176.3530181846559], [8, 219.25862916727175]], "LATENCY": [[1, 29.500679969787594], [2, 31.625401973724365], [4, 37.555546760559075], [8, 51.32622241973876]]}}}</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{"Classifier-resnet34/prepoc-resnet34": {"CPU1": {"THROUGHPUT": [[1, 118.31185229026288], [2, 157.66939867806386], [4, 164.02599009533154], [8, 150.10035310033894]], "LATENCY": [[1, 19.894261360168457], [2, 30.623347759246823], [4, 54.12736415863037], [8, 96.48118734359741]]}}, "Classifier-resnet34/model-resnet34": {"Tesla P40": {"THROUGHPUT": [[1, 97.03822580153341], [2, 147.0392391028999], [4, 180.975479470437], [8, 210.34197702313352]], "LATENCY": [[1, 25.29911756515503], [2, 26.919329166412354], [4, 33.29339265823364], [8, 43.86476755142211]]}}}</t>
+          <t>{"Classifier-resnet34/prepoc-resnet34": {"CPU1": {"THROUGHPUT": [[1, 107.72191494622872], [2, 141.0505317091839], [4, 137.39671424865102], [8, 133.88230676603754]], "LATENCY": [[1, 19.885082244873043], [2, 31.806173324584957], [4, 51.76976203918457], [8, 98.1454586982727]]}}, "Classifier-resnet34/model-resnet34": {"Tesla P40": {"THROUGHPUT": [[1, 97.08632510682425], [2, 139.43258706957215], [4, 171.55825862255003], [8, 225.5949406713249]], "LATENCY": [[1, 24.84185218811035], [2, 28.206875324249264], [4, 33.457314968109124], [8, 50.905413627624505]]}}}</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1211,7 +1211,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>72.40000000000001</v>
+        <v>75.8</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>

</xml_diff>